<commit_message>
:recycle: [Refactor] InitData Refact
</commit_message>
<xml_diff>
--- a/src/main/resources/file/RoadMap-CS-Quiz.xlsx
+++ b/src/main/resources/file/RoadMap-CS-Quiz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaehyun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaehyun/Documents/IdeaProjects/KaKaoCloud/Project/Second/BackEndRoadMap/src/main/resources/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF15C8-543D-D745-B136-F8758EAA29D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CDB116-19F1-3E48-AC96-AEBC1860BFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{80011468-7F19-A742-8D0A-556DCE69D518}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>대분류 FK</t>
   </si>
@@ -303,10 +303,6 @@
   </si>
   <si>
     <t>해설없음</t>
-  </si>
-  <si>
-    <t>ㄷ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>서버는 클라이언트에 결과를 반환한다.</t>
@@ -334,10 +330,6 @@
     <t>CSS는 웹페이지를 꾸미기 위한 Style sheet 언어이다.</t>
   </si>
   <si>
-    <t>ㄹ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Java Script는 서버측에서 실행되는 객체 기반 언어이다.</t>
   </si>
   <si>
@@ -353,15 +345,7 @@
     <t>운영 체제는 사용자가 컴퓨터 하드웨어 간의 인터페이스를 제공해 주는 프로그램</t>
   </si>
   <si>
-    <t>ㅁ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>저장 공간 자동 정리 기능은 운영체제 기능이 아니다.</t>
-  </si>
-  <si>
-    <t>ㄱ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>프로세스는 CPU에 의해서 현재 실행되고 있는 프로그램을 의미한다.</t>
@@ -383,6 +367,61 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>C언어는 절차지향 언어이다.</t>
+  </si>
+  <si>
+    <t>한정된 객체와 객체 함수를 제공한다.</t>
+  </si>
+  <si>
+    <t>Go는 LG에서 개발한 컴파일 언어로, 간결한 문법과 빠른 컴파일 속도, 직렬 프로그래밍을 위한 지원 등을 특징으로 한다.</t>
+  </si>
+  <si>
+    <t>Go는 google에서 개발한 컴파일 언어이며, 병렬 프로그래밍을 위한 지원 등을 특징으로 한다.</t>
+  </si>
+  <si>
+    <t>PHP는 ‘Personal Hypertext Tools’의 약자로 웹사이트 제작에 특화된 벡엔드(서버) 언어로 동적 웹 페이지 생성 및 데이터베이스 상호작용을 위한 내장 지원을 제공한다.</t>
+  </si>
+  <si>
+    <t>INTERNET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BASIC_FE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>클라이언트는 서버에 결과에 반환한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>"&lt;wgroup&gt;"는 HTML의 태그이다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>운영체제의 기능 중 하나로 "저장 공간 자동 정리"이 있다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C언어는 객체지향언어가 아니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>JavaScript는 제한된 객체와 객체 함수를 제공한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Process의 특징 중 하나로 프로세스는 메모리에 의해서 현재 실행되고 있는 프로그램을 의미한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -476,16 +515,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>ㅁ소드를</t>
+      <t xml:space="preserve"> 메</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>소드를</t>
     </r>
     <r>
       <rPr>
@@ -792,966 +831,6 @@
       </rPr>
       <t>기술</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>C언어는 절차지향 언어이다.</t>
-  </si>
-  <si>
-    <t>한정된 객체와 객체 함수를 제공한다.</t>
-  </si>
-  <si>
-    <t>Go는 LG에서 개발한 컴파일 언어로, 간결한 문법과 빠른 컴파일 속도, 직렬 프로그래밍을 위한 지원 등을 특징으로 한다.</t>
-  </si>
-  <si>
-    <t>Go는 google에서 개발한 컴파일 언어이며, 병렬 프로그래밍을 위한 지원 등을 특징으로 한다.</t>
-  </si>
-  <si>
-    <t>PHP는 ‘Personal Hypertext Tools’의 약자로 웹사이트 제작에 특화된 벡엔드(서버) 언어로 동적 웹 페이지 생성 및 데이터베이스 상호작용을 위한 내장 지원을 제공한다.</t>
-  </si>
-  <si>
-    <t>INTERNET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BASIC_FE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LANGUAGE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HTTP의 특징중에 옳은것은?&lt;br/&gt;
-ㄱ. 클라이언트 서버구조&lt;br/&gt;
-ㄴ. Stateless 무상태 프로토콜&lt;br/&gt;
-ㄷ. 클라이언트는 서버에 결과에 반환&lt;br/&gt;
-ㄹ. 서버는 클라이언트의 상태보존을 하지 않는다&lt;br/&gt;
-ㅁ. 저장 공간 자동 정리&lt;br/&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>운영체제의 기능이 아닌 것은? &lt;br/&gt;
-ㄱ. 컴퓨터 자원 관리&lt;br/&gt;
-ㄴ. 하드웨어의 고장 탐색 및 오류 처리&lt;br/&gt;
-ㄷ. 컴퓨터 자원 보호 및 보안 관리&lt;br/&gt;
-ㄹ. 사용자에게 편리한 인터페이스 제공&lt;br/&gt;
-ㅁ. 저장 공간 자동 정리&lt;br/&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Process의 특징으로 틀린 것은?&lt;br/&gt;
-ㄱ. 프로세스는 메모리에 의해서 현재 실행되고 있는 프로그램을 의미한다.&lt;br/&gt;
-ㄴ. 프로세스 스케줄링은 프로세스들 사이의 우선순위를 관리하고 시스템의 자원을 해당 프로세스에게 할당하는 작업을 의미한다.&lt;br/&gt;
-ㄷ. 선입선처리(First Come First Served) 스케줄링이란 스케줄링은 CPU에 먼저 도착하는 순서대로 프로세스를 할당해 실행하는 방식이다.&lt;br/&gt;
-ㄹ. 최단 작업 우선(Short Job First) 스케줄링이란 작업이 끝나기까지의 실행 시간 추정치가 가장 작은 작업을 먼저 실행시키는 방식이다.&lt;br/&gt;
-ㅁ. 라운드 로빈(Round Robin) 스케줄링이란 동일한 시간 할당량을 사용하는 시분할 처리 방식이다.&lt;br/&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>객체지향언어가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>아닌</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>것은</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?&lt;br/&gt;
-ㄱ. JAVA&lt;br/&gt;
-ㄴ. C++&lt;br/&gt;
-ㄷ. Ruby&lt;br/&gt;
-ㄹ. Python&lt;br/&gt;
-ㅁ. C&lt;br/&gt;</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>JavaScript</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>특징으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>틀린</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>것은</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">?&lt;br/&gt;
-ㄱ. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>컴파일</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>과정이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>필요</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>없으므로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>빠른</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>시간</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>안에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>스크립트</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>코드를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>작성할</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>있다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.&lt;br/&gt;
-ㄴ. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>웹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>브라우저에서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>기본적으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>실행되며</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>다양한</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>라이브러리와</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>프레임워크를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>제공한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.&lt;br/&gt;
-ㄷ. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>다양한</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>플랫폼에서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>실행</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>가능하며</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>비동기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>프로그래밍을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>지원한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.&lt;br/&gt;
-ㄹ. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>동적</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>타이핑으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>인한</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>버그</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>발생</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>가능성이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>있다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.&lt;br/&gt;
-ㅁ. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>제한된</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>객체와</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>객체</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>함수를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-      </rPr>
-      <t>제공한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.&lt;br/&gt;</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음 중 HTML의 태그가 아닌 것은?&lt;br/&gt;
-ㄱ. "&lt;div&gt;"&lt;br/&gt;
-ㄴ. "&lt;nav&gt;"&lt;br/&gt;
-ㄷ. "&lt;hgroup&gt;"&lt;br/&gt;
-ㄹ. "&lt;wgroup&gt;"&lt;br/&gt;
-ㅁ. "&lt;article&gt;"&lt;br/&gt;</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1951,11 +1030,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2293,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767C6903-E409-C549-987D-3AE3151DDC9F}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2320,7 +1399,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -2334,7 +1413,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -2348,7 +1427,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -2360,236 +1439,236 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="96">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="96">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="96">
-      <c r="A13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="112">
-      <c r="A14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="96">
       <c r="A17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="96">
-      <c r="A18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="96">
-      <c r="A19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>27</v>
+      <c r="C19" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>

</xml_diff>